<commit_message>
Beta share holdings extraction completed.
</commit_message>
<xml_diff>
--- a/scripts/BetaShares List.xlsx
+++ b/scripts/BetaShares List.xlsx
@@ -5,20 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\Python Scripts\ETF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\GitHub\etftracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760A3BA6-4F09-4339-8532-752E7F6EDDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AADA6F-6F81-4601-BAC0-A8AFA95BF837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4EA49AC6-DA87-479A-8452-29EDAED46CE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Fixed Income" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$56</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="376">
   <si>
     <t>ASX Code</t>
   </si>
@@ -3530,11 +3534,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916DDE32-C910-40C7-87DB-77EF5DC70101}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D60"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3559,76 +3561,76 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>VLOOKUP(B2,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia</v>
+        <v>Cash</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
         <v>308</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>VLOOKUP(B3,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Cash</v>
+        <v>Commodity</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D3" t="s">
-        <v>311</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>VLOOKUP(B4,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Fixed Income - Australia Dollar</v>
+        <v>Commodity</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>251</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
         <v>309</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>VLOOKUP(B5,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Asia</v>
+        <v>Currency</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C5" t="s">
         <v>309</v>
       </c>
       <c r="D5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>VLOOKUP(B6,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Sectors</v>
+        <v>Currency</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
         <v>309</v>
       </c>
       <c r="D6" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3637,403 +3639,403 @@
         <v>Currency</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>254</v>
+        <v>293</v>
       </c>
       <c r="C7" t="s">
         <v>309</v>
       </c>
       <c r="D7" t="s">
-        <v>315</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>VLOOKUP(B8,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
+        <v>Currency</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>255</v>
+        <v>304</v>
       </c>
       <c r="C8" t="s">
         <v>309</v>
       </c>
       <c r="D8" t="s">
-        <v>316</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>VLOOKUP(B9,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
+        <v>Currency</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>256</v>
+        <v>306</v>
       </c>
       <c r="C9" t="s">
         <v>309</v>
       </c>
       <c r="D9" t="s">
-        <v>317</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>VLOOKUP(B10,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
+        <v>Equity - Asia</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C10" t="s">
         <v>309</v>
       </c>
       <c r="D10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>VLOOKUP(B11,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
+        <v>Equity - Asia</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="C11" t="s">
         <v>309</v>
       </c>
       <c r="D11" t="s">
-        <v>319</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>VLOOKUP(B12,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Fixed Income - Australia Dollar</v>
+        <v>Equity - Asia</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
       <c r="C12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D12" t="s">
-        <v>320</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>VLOOKUP(B13,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Fixed Income - Australia Dollar</v>
+        <v>Equity - Australia</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D13" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>VLOOKUP(B14,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Sectors</v>
+        <v>Equity - Australia</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>261</v>
+        <v>297</v>
       </c>
       <c r="C14" t="s">
         <v>309</v>
       </c>
       <c r="D14" t="s">
-        <v>322</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>VLOOKUP(B15,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
+        <v>Equity - Australia Sectors</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C15" t="s">
         <v>309</v>
       </c>
       <c r="D15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>VLOOKUP(B16,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Fixed Income - Australia Dollar</v>
+        <v>Equity - Australia Sectors</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>263</v>
+        <v>295</v>
       </c>
       <c r="C16" t="s">
         <v>309</v>
       </c>
       <c r="D16" t="s">
-        <v>324</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>VLOOKUP(B17,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Mixed Asset</v>
+        <v>Equity - Australia Sectors</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="C17" t="s">
         <v>309</v>
       </c>
       <c r="D17" t="s">
-        <v>325</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>VLOOKUP(B18,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Mixed Asset</v>
+        <v>Equity - Australia Small/Mid Cap</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C18" t="s">
         <v>309</v>
       </c>
       <c r="D18" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>VLOOKUP(B19,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Mixed Asset</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C19" t="s">
         <v>309</v>
       </c>
       <c r="D19" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>VLOOKUP(B20,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Sectors</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C20" t="s">
         <v>309</v>
       </c>
       <c r="D20" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>VLOOKUP(B21,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Mixed Asset</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C21" t="s">
         <v>309</v>
       </c>
       <c r="D21" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>VLOOKUP(B22,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Currency</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C22" t="s">
         <v>309</v>
       </c>
       <c r="D22" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>VLOOKUP(B23,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="C23" t="s">
         <v>309</v>
       </c>
       <c r="D23" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>VLOOKUP(B24,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="C24" t="s">
         <v>309</v>
       </c>
       <c r="D24" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>VLOOKUP(B25,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Small/Mid Cap</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="C25" t="s">
         <v>309</v>
       </c>
       <c r="D25" t="s">
-        <v>333</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>VLOOKUP(B26,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global</v>
+        <v>Equity - Australia Strategy</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="C26" t="s">
         <v>309</v>
       </c>
       <c r="D26" t="s">
-        <v>334</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>VLOOKUP(B27,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
+        <v>Equity - Global</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C27" t="s">
         <v>309</v>
       </c>
       <c r="D27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>VLOOKUP(B28,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Sectors</v>
+        <v>Equity - Global</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C28" t="s">
         <v>309</v>
       </c>
       <c r="D28" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>VLOOKUP(B29,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Sectors</v>
+        <v>Equity - Global</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="C29" t="s">
         <v>309</v>
       </c>
       <c r="D29" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>VLOOKUP(B30,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Fixed Income - Global</v>
+        <v>Equity - Global</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C30" t="s">
         <v>309</v>
       </c>
       <c r="D30" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>VLOOKUP(B31,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
+        <v>Equity - Global</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="C31" t="s">
         <v>309</v>
       </c>
       <c r="D31" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>VLOOKUP(B32,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Fixed Income - Global</v>
+        <v>Equity - Global</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="C32" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D32" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>VLOOKUP(B33,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
+        <v>Equity - Global Sectors</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="C33" t="s">
         <v>309</v>
       </c>
       <c r="D33" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4042,118 +4044,118 @@
         <v>Equity - Global Sectors</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C34" t="s">
         <v>309</v>
       </c>
       <c r="D34" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>VLOOKUP(B35,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
+        <v>Equity - Global Sectors</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C35" t="s">
         <v>309</v>
       </c>
       <c r="D35" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>VLOOKUP(B36,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global</v>
+        <v>Equity - Global Sectors</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C36" t="s">
         <v>309</v>
       </c>
       <c r="D36" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>VLOOKUP(B37,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Asia</v>
+        <v>Equity - Global Sectors</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C37" t="s">
         <v>309</v>
       </c>
       <c r="D37" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>VLOOKUP(B38,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global</v>
+        <v>Equity - Global Sectors</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C38" t="s">
         <v>309</v>
       </c>
       <c r="D38" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>VLOOKUP(B39,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
+        <v>Equity - Global Sectors</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="C39" t="s">
         <v>309</v>
       </c>
       <c r="D39" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>VLOOKUP(B40,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="C40" t="s">
         <v>309</v>
       </c>
       <c r="D40" t="s">
-        <v>348</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>VLOOKUP(B41,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Asia</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="C41" t="s">
         <v>309</v>
       </c>
       <c r="D41" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4162,103 +4164,103 @@
         <v>Equity - Global Strategy</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="C42" t="s">
         <v>309</v>
       </c>
       <c r="D42" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>VLOOKUP(B43,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Sectors</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="C43" t="s">
         <v>309</v>
       </c>
       <c r="D43" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>VLOOKUP(B44,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C44" t="s">
         <v>309</v>
       </c>
       <c r="D44" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>VLOOKUP(B45,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Commodity</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="C45" t="s">
         <v>309</v>
       </c>
       <c r="D45" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>VLOOKUP(B46,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Currency</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C46" t="s">
         <v>309</v>
       </c>
       <c r="D46" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>VLOOKUP(B47,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Commodity</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C47" t="s">
         <v>309</v>
       </c>
       <c r="D47" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>VLOOKUP(B48,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Sectors</v>
+        <v>Equity - Global Strategy</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C48" t="s">
         <v>309</v>
       </c>
       <c r="D48" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4267,181 +4269,81 @@
         <v>Equity - Global Strategy</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="C49" t="s">
         <v>309</v>
       </c>
       <c r="D49" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>VLOOKUP(B50,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia</v>
+        <v>Mixed Asset</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>297</v>
+        <v>264</v>
       </c>
       <c r="C50" t="s">
         <v>309</v>
       </c>
       <c r="D50" t="s">
-        <v>358</v>
+        <v>325</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>VLOOKUP(B51,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Fixed Income - Australia Dollar</v>
+        <v>Mixed Asset</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>298</v>
+        <v>265</v>
       </c>
       <c r="C51" t="s">
         <v>309</v>
       </c>
       <c r="D51" t="s">
-        <v>359</v>
+        <v>326</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>VLOOKUP(B52,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Sectors</v>
+        <v>Mixed Asset</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>299</v>
+        <v>266</v>
       </c>
       <c r="C52" t="s">
         <v>309</v>
       </c>
       <c r="D52" t="s">
-        <v>360</v>
+        <v>327</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>VLOOKUP(B53,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global</v>
+        <v>Mixed Asset</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="C53" t="s">
         <v>309</v>
       </c>
       <c r="D53" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
-        <f>VLOOKUP(B54,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Sectors</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="C54" t="s">
-        <v>309</v>
-      </c>
-      <c r="D54" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="str">
-        <f>VLOOKUP(B55,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="C55" t="s">
-        <v>309</v>
-      </c>
-      <c r="D55" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="str">
-        <f>VLOOKUP(B56,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global Strategy</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="C56" t="s">
-        <v>309</v>
-      </c>
-      <c r="D56" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="str">
-        <f>VLOOKUP(B57,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Currency</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="C57" t="s">
-        <v>309</v>
-      </c>
-      <c r="D57" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
-        <f>VLOOKUP(B58,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Global</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="C58" t="s">
-        <v>309</v>
-      </c>
-      <c r="D58" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
-        <f>VLOOKUP(B59,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Currency</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="C59" t="s">
-        <v>309</v>
-      </c>
-      <c r="D59" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="str">
-        <f>VLOOKUP(B60,[1]Sheet1!$B:$C,2,FALSE)</f>
-        <v>Equity - Australia Strategy</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="C60" t="s">
-        <v>309</v>
-      </c>
-      <c r="D60" t="s">
-        <v>368</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D60" xr:uid="{916DDE32-C910-40C7-87DB-77EF5DC70101}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">
+      <sortCondition ref="A1:A60"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7196,4 +7098,138 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902974F3-FB8E-42D4-84D9-A0D7E2C4548D}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>VLOOKUP(B2,[1]Sheet1!$B:$C,2,FALSE)</f>
+        <v>Fixed Income - Australia Dollar</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>VLOOKUP(B3,[1]Sheet1!$B:$C,2,FALSE)</f>
+        <v>Fixed Income - Australia Dollar</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>VLOOKUP(B4,[1]Sheet1!$B:$C,2,FALSE)</f>
+        <v>Fixed Income - Australia Dollar</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>VLOOKUP(B5,[1]Sheet1!$B:$C,2,FALSE)</f>
+        <v>Fixed Income - Australia Dollar</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>VLOOKUP(B6,[1]Sheet1!$B:$C,2,FALSE)</f>
+        <v>Fixed Income - Australia Dollar</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>VLOOKUP(B7,[1]Sheet1!$B:$C,2,FALSE)</f>
+        <v>Fixed Income - Global</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>VLOOKUP(B8,[1]Sheet1!$B:$C,2,FALSE)</f>
+        <v>Fixed Income - Global</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>